<commit_message>
update JDD + tests Azure
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.MAT.xlsx
+++ b/TNR_JDD/JDD.RT.MAT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="616">
   <si>
     <t>Date</t>
   </si>
@@ -1535,9 +1535,6 @@
   </si>
   <si>
     <t>CAL.RT.MAT.001.CRE.02</t>
-  </si>
-  <si>
-    <t>EMP.RT.MAT.001.CRE.02.........</t>
   </si>
   <si>
     <t>GROUPE02</t>
@@ -9669,7 +9666,7 @@
         <v>45658.0</v>
       </c>
       <c r="W8" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X8" s="62">
         <v>44593.0</v>
@@ -9824,14 +9821,14 @@
       <c r="BV8" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW8" s="61" t="s">
-        <v>373</v>
+      <c r="BW8" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX8" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY8" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ8" s="62">
         <v>44562.0</v>
@@ -10007,14 +10004,14 @@
       <c r="T9" s="12">
         <v>20000.0</v>
       </c>
-      <c r="U9" s="12" t="s">
-        <v>365</v>
+      <c r="U9" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V9" s="62">
         <v>45658.0</v>
       </c>
       <c r="W9" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X9" s="62">
         <v>44593.0</v>
@@ -10098,13 +10095,13 @@
         <v>374</v>
       </c>
       <c r="AY9" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="AZ9" s="60" t="s">
         <v>399</v>
       </c>
-      <c r="AZ9" s="60" t="s">
+      <c r="BA9" s="12" t="s">
         <v>400</v>
-      </c>
-      <c r="BA9" s="12" t="s">
-        <v>401</v>
       </c>
       <c r="BB9" s="62">
         <v>44562.0</v>
@@ -10134,16 +10131,16 @@
         <v>365</v>
       </c>
       <c r="BK9" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="BL9" s="12">
         <v>2.0</v>
       </c>
       <c r="BM9" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="BN9" s="12" t="s">
         <v>403</v>
-      </c>
-      <c r="BN9" s="12" t="s">
-        <v>404</v>
       </c>
       <c r="BO9" s="12" t="s">
         <v>365</v>
@@ -10161,22 +10158,22 @@
         <v>365</v>
       </c>
       <c r="BT9" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="BU9" s="34" t="s">
         <v>405</v>
-      </c>
-      <c r="BU9" s="34" t="s">
-        <v>406</v>
       </c>
       <c r="BV9" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW9" s="61" t="s">
-        <v>373</v>
+      <c r="BW9" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX9" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY9" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ9" s="62">
         <v>44562.0</v>
@@ -10203,34 +10200,34 @@
         <v>365</v>
       </c>
       <c r="CH9" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="CI9" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="CJ9" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="CK9" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="CL9" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="CI9" s="29" t="s">
+      <c r="CM9" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="CJ9" s="29" t="s">
+      <c r="CN9" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="CK9" s="29" t="s">
+      <c r="CO9" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="CL9" s="57" t="s">
+      <c r="CP9" s="57" t="s">
+        <v>405</v>
+      </c>
+      <c r="CQ9" s="12" t="s">
         <v>408</v>
-      </c>
-      <c r="CM9" s="57" t="s">
-        <v>408</v>
-      </c>
-      <c r="CN9" s="57" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO9" s="57" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP9" s="57" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ9" s="12" t="s">
-        <v>409</v>
       </c>
       <c r="CR9" s="62">
         <v>44227.0</v>
@@ -10242,7 +10239,7 @@
         <v>366</v>
       </c>
       <c r="CU9" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="CV9" s="12" t="s">
         <v>365</v>
@@ -10276,7 +10273,7 @@
       <c r="DQ9" s="64"/>
       <c r="DR9" s="64"/>
       <c r="DS9" s="40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="DT9" s="40" t="s">
         <v>397</v>
@@ -10290,15 +10287,15 @@
       <c r="DX9" s="64"/>
       <c r="DY9" s="64"/>
       <c r="DZ9" s="66" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>365</v>
@@ -10307,7 +10304,7 @@
         <v>363</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>365</v>
@@ -10328,16 +10325,16 @@
         <v>367</v>
       </c>
       <c r="L10" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N10" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>416</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>417</v>
       </c>
       <c r="P10" s="60" t="s">
         <v>371</v>
@@ -10349,19 +10346,19 @@
         <v>365</v>
       </c>
       <c r="S10" s="35" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T10" s="12">
         <v>30000.0</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>365</v>
+      <c r="U10" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V10" s="62">
         <v>45658.0</v>
       </c>
       <c r="W10" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X10" s="62">
         <v>44593.0</v>
@@ -10400,7 +10397,7 @@
         <v>365</v>
       </c>
       <c r="AJ10" s="57" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AK10" s="12" t="s">
         <v>365</v>
@@ -10418,7 +10415,7 @@
         <v>30000.0</v>
       </c>
       <c r="AP10" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AQ10" s="12" t="s">
         <v>377</v>
@@ -10448,10 +10445,10 @@
         <v>365</v>
       </c>
       <c r="AZ10" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="BA10" s="12" t="s">
         <v>421</v>
-      </c>
-      <c r="BA10" s="12" t="s">
-        <v>422</v>
       </c>
       <c r="BB10" s="62">
         <v>44562.0</v>
@@ -10481,16 +10478,16 @@
         <v>365</v>
       </c>
       <c r="BK10" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="BL10" s="12">
         <v>3.0</v>
       </c>
       <c r="BM10" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="BN10" s="12" t="s">
         <v>424</v>
-      </c>
-      <c r="BN10" s="12" t="s">
-        <v>425</v>
       </c>
       <c r="BO10" s="12" t="s">
         <v>365</v>
@@ -10508,22 +10505,22 @@
         <v>365</v>
       </c>
       <c r="BT10" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="BU10" s="34" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="BV10" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW10" s="61" t="s">
-        <v>373</v>
+      <c r="BW10" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX10" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY10" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ10" s="62">
         <v>44562.0</v>
@@ -10550,34 +10547,34 @@
         <v>365</v>
       </c>
       <c r="CH10" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CI10" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CJ10" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CK10" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CL10" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="CI10" s="29" t="s">
+      <c r="CM10" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="CJ10" s="29" t="s">
+      <c r="CN10" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="CK10" s="29" t="s">
+      <c r="CO10" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="CL10" s="57" t="s">
+      <c r="CP10" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="CQ10" s="12" t="s">
         <v>428</v>
-      </c>
-      <c r="CM10" s="57" t="s">
-        <v>428</v>
-      </c>
-      <c r="CN10" s="57" t="s">
-        <v>428</v>
-      </c>
-      <c r="CO10" s="57" t="s">
-        <v>428</v>
-      </c>
-      <c r="CP10" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="CQ10" s="12" t="s">
-        <v>429</v>
       </c>
       <c r="CR10" s="62">
         <v>44227.0</v>
@@ -10589,7 +10586,7 @@
         <v>366</v>
       </c>
       <c r="CU10" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="CV10" s="12" t="s">
         <v>365</v>
@@ -10623,10 +10620,10 @@
       <c r="DQ10" s="64"/>
       <c r="DR10" s="64"/>
       <c r="DS10" s="40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="DT10" s="40" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="DU10" s="64"/>
       <c r="DV10" s="64"/>
@@ -10637,15 +10634,15 @@
       <c r="DX10" s="64"/>
       <c r="DY10" s="64"/>
       <c r="DZ10" s="66" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="56" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>365</v>
@@ -10654,7 +10651,7 @@
         <v>363</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>365</v>
@@ -10675,16 +10672,16 @@
         <v>367</v>
       </c>
       <c r="L11" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N11" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>436</v>
       </c>
       <c r="P11" s="60" t="s">
         <v>371</v>
@@ -10701,14 +10698,14 @@
       <c r="T11" s="12">
         <v>40000.0</v>
       </c>
-      <c r="U11" s="12" t="s">
-        <v>365</v>
+      <c r="U11" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V11" s="62">
         <v>45658.0</v>
       </c>
       <c r="W11" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X11" s="62">
         <v>44593.0</v>
@@ -10765,7 +10762,7 @@
         <v>40000.0</v>
       </c>
       <c r="AP11" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AQ11" s="12" t="s">
         <v>377</v>
@@ -10798,7 +10795,7 @@
         <v>378</v>
       </c>
       <c r="BA11" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB11" s="62">
         <v>44562.0</v>
@@ -10828,13 +10825,13 @@
         <v>365</v>
       </c>
       <c r="BK11" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="BL11" s="12">
         <v>1.0</v>
       </c>
       <c r="BM11" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BN11" s="12" t="s">
         <v>382</v>
@@ -10855,22 +10852,22 @@
         <v>365</v>
       </c>
       <c r="BT11" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="BU11" s="34" t="s">
         <v>441</v>
-      </c>
-      <c r="BU11" s="34" t="s">
-        <v>442</v>
       </c>
       <c r="BV11" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW11" s="61" t="s">
-        <v>373</v>
+      <c r="BW11" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX11" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY11" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ11" s="62">
         <v>44562.0</v>
@@ -10897,34 +10894,34 @@
         <v>365</v>
       </c>
       <c r="CH11" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="CI11" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="CJ11" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="CK11" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="CL11" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="CI11" s="29" t="s">
+      <c r="CM11" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="CJ11" s="29" t="s">
+      <c r="CN11" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="CK11" s="29" t="s">
+      <c r="CO11" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="CL11" s="57" t="s">
+      <c r="CP11" s="57" t="s">
+        <v>441</v>
+      </c>
+      <c r="CQ11" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="CM11" s="57" t="s">
-        <v>444</v>
-      </c>
-      <c r="CN11" s="57" t="s">
-        <v>444</v>
-      </c>
-      <c r="CO11" s="57" t="s">
-        <v>444</v>
-      </c>
-      <c r="CP11" s="57" t="s">
-        <v>442</v>
-      </c>
-      <c r="CQ11" s="12" t="s">
-        <v>445</v>
       </c>
       <c r="CR11" s="62">
         <v>44227.0</v>
@@ -10970,7 +10967,7 @@
       <c r="DQ11" s="64"/>
       <c r="DR11" s="64"/>
       <c r="DS11" s="40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="DT11" s="40" t="s">
         <v>363</v>
@@ -10984,15 +10981,15 @@
       </c>
       <c r="DY11" s="65"/>
       <c r="DZ11" s="66" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="56" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>365</v>
@@ -11001,7 +10998,7 @@
         <v>363</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>365</v>
@@ -11022,16 +11019,16 @@
         <v>367</v>
       </c>
       <c r="L12" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N12" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>450</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>451</v>
       </c>
       <c r="P12" s="60" t="s">
         <v>371</v>
@@ -11048,14 +11045,14 @@
       <c r="T12" s="12">
         <v>50000.0</v>
       </c>
-      <c r="U12" s="12" t="s">
-        <v>365</v>
+      <c r="U12" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V12" s="62">
         <v>45658.0</v>
       </c>
       <c r="W12" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X12" s="62">
         <v>44593.0</v>
@@ -11112,7 +11109,7 @@
         <v>50000.0</v>
       </c>
       <c r="AP12" s="12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AQ12" s="12" t="s">
         <v>374</v>
@@ -11142,10 +11139,10 @@
         <v>365</v>
       </c>
       <c r="AZ12" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BA12" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="BB12" s="62">
         <v>44562.0</v>
@@ -11175,16 +11172,16 @@
         <v>365</v>
       </c>
       <c r="BK12" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="BL12" s="12">
         <v>2.0</v>
       </c>
       <c r="BM12" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BN12" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="BO12" s="12" t="s">
         <v>365</v>
@@ -11202,22 +11199,22 @@
         <v>365</v>
       </c>
       <c r="BT12" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="BU12" s="34" t="s">
         <v>456</v>
-      </c>
-      <c r="BU12" s="34" t="s">
-        <v>457</v>
       </c>
       <c r="BV12" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW12" s="61" t="s">
-        <v>373</v>
+      <c r="BW12" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX12" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY12" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ12" s="62">
         <v>44562.0</v>
@@ -11244,34 +11241,34 @@
         <v>365</v>
       </c>
       <c r="CH12" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="CI12" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="CJ12" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="CK12" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="CL12" s="57" t="s">
         <v>458</v>
       </c>
-      <c r="CI12" s="29" t="s">
+      <c r="CM12" s="57" t="s">
         <v>458</v>
       </c>
-      <c r="CJ12" s="29" t="s">
+      <c r="CN12" s="57" t="s">
         <v>458</v>
       </c>
-      <c r="CK12" s="29" t="s">
+      <c r="CO12" s="57" t="s">
         <v>458</v>
       </c>
-      <c r="CL12" s="57" t="s">
+      <c r="CP12" s="57" t="s">
+        <v>456</v>
+      </c>
+      <c r="CQ12" s="12" t="s">
         <v>459</v>
-      </c>
-      <c r="CM12" s="57" t="s">
-        <v>459</v>
-      </c>
-      <c r="CN12" s="57" t="s">
-        <v>459</v>
-      </c>
-      <c r="CO12" s="57" t="s">
-        <v>459</v>
-      </c>
-      <c r="CP12" s="57" t="s">
-        <v>457</v>
-      </c>
-      <c r="CQ12" s="12" t="s">
-        <v>460</v>
       </c>
       <c r="CR12" s="62">
         <v>44227.0</v>
@@ -11283,7 +11280,7 @@
         <v>366</v>
       </c>
       <c r="CU12" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="CV12" s="12" t="s">
         <v>365</v>
@@ -11317,7 +11314,7 @@
       <c r="DQ12" s="64"/>
       <c r="DR12" s="64"/>
       <c r="DS12" s="40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="DT12" s="40" t="s">
         <v>363</v>
@@ -11331,15 +11328,15 @@
       </c>
       <c r="DY12" s="64"/>
       <c r="DZ12" s="66" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>365</v>
@@ -11348,7 +11345,7 @@
         <v>363</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>365</v>
@@ -11369,16 +11366,16 @@
         <v>367</v>
       </c>
       <c r="L13" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N13" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="M13" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N13" s="12" t="s">
+      <c r="O13" s="12" t="s">
         <v>465</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>466</v>
       </c>
       <c r="P13" s="60" t="s">
         <v>371</v>
@@ -11395,14 +11392,14 @@
       <c r="T13" s="12">
         <v>60000.0</v>
       </c>
-      <c r="U13" s="12" t="s">
-        <v>365</v>
+      <c r="U13" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V13" s="62">
         <v>45658.0</v>
       </c>
       <c r="W13" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X13" s="62">
         <v>44593.0</v>
@@ -11459,7 +11456,7 @@
         <v>60000.0</v>
       </c>
       <c r="AP13" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AQ13" s="12" t="s">
         <v>377</v>
@@ -11489,10 +11486,10 @@
         <v>365</v>
       </c>
       <c r="AZ13" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BA13" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="BB13" s="62">
         <v>44562.0</v>
@@ -11522,16 +11519,16 @@
         <v>365</v>
       </c>
       <c r="BK13" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="BL13" s="12">
         <v>3.0</v>
       </c>
       <c r="BM13" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="BN13" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BO13" s="12" t="s">
         <v>365</v>
@@ -11549,22 +11546,22 @@
         <v>365</v>
       </c>
       <c r="BT13" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="BU13" s="34" t="s">
         <v>471</v>
-      </c>
-      <c r="BU13" s="34" t="s">
-        <v>472</v>
       </c>
       <c r="BV13" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW13" s="61" t="s">
-        <v>373</v>
+      <c r="BW13" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX13" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY13" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ13" s="62">
         <v>44562.0</v>
@@ -11591,34 +11588,34 @@
         <v>365</v>
       </c>
       <c r="CH13" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="CI13" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="CJ13" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="CK13" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="CL13" s="57" t="s">
         <v>473</v>
       </c>
-      <c r="CI13" s="29" t="s">
+      <c r="CM13" s="57" t="s">
         <v>473</v>
       </c>
-      <c r="CJ13" s="29" t="s">
+      <c r="CN13" s="57" t="s">
         <v>473</v>
       </c>
-      <c r="CK13" s="29" t="s">
+      <c r="CO13" s="57" t="s">
         <v>473</v>
       </c>
-      <c r="CL13" s="57" t="s">
+      <c r="CP13" s="57" t="s">
+        <v>471</v>
+      </c>
+      <c r="CQ13" s="12" t="s">
         <v>474</v>
-      </c>
-      <c r="CM13" s="57" t="s">
-        <v>474</v>
-      </c>
-      <c r="CN13" s="57" t="s">
-        <v>474</v>
-      </c>
-      <c r="CO13" s="57" t="s">
-        <v>474</v>
-      </c>
-      <c r="CP13" s="57" t="s">
-        <v>472</v>
-      </c>
-      <c r="CQ13" s="12" t="s">
-        <v>475</v>
       </c>
       <c r="CR13" s="62">
         <v>44227.0</v>
@@ -11630,7 +11627,7 @@
         <v>366</v>
       </c>
       <c r="CU13" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="CV13" s="12" t="s">
         <v>365</v>
@@ -11671,15 +11668,15 @@
       <c r="DX13" s="64"/>
       <c r="DY13" s="64"/>
       <c r="DZ13" s="66" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="56" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>365</v>
@@ -11688,7 +11685,7 @@
         <v>363</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>365</v>
@@ -11709,16 +11706,16 @@
         <v>367</v>
       </c>
       <c r="L14" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N14" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="M14" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N14" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>480</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>481</v>
       </c>
       <c r="P14" s="60" t="s">
         <v>371</v>
@@ -11735,14 +11732,14 @@
       <c r="T14" s="12">
         <v>70000.0</v>
       </c>
-      <c r="U14" s="12" t="s">
-        <v>365</v>
+      <c r="U14" s="61" t="s">
+        <v>373</v>
       </c>
       <c r="V14" s="62">
         <v>45658.0</v>
       </c>
       <c r="W14" s="61" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="X14" s="62">
         <v>44593.0</v>
@@ -11799,7 +11796,7 @@
         <v>70000.0</v>
       </c>
       <c r="AP14" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AQ14" s="12" t="s">
         <v>377</v>
@@ -11829,10 +11826,10 @@
         <v>365</v>
       </c>
       <c r="AZ14" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BA14" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="BB14" s="62">
         <v>44562.0</v>
@@ -11862,16 +11859,16 @@
         <v>365</v>
       </c>
       <c r="BK14" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="BL14" s="12">
         <v>3.0</v>
       </c>
       <c r="BM14" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="BN14" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BO14" s="12" t="s">
         <v>365</v>
@@ -11889,22 +11886,22 @@
         <v>365</v>
       </c>
       <c r="BT14" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="BU14" s="34" t="s">
         <v>486</v>
-      </c>
-      <c r="BU14" s="34" t="s">
-        <v>487</v>
       </c>
       <c r="BV14" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="BW14" s="61" t="s">
-        <v>373</v>
+      <c r="BW14" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="BX14" s="35" t="s">
         <v>375</v>
       </c>
       <c r="BY14" s="35" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="BZ14" s="62">
         <v>44562.0</v>
@@ -11931,34 +11928,34 @@
         <v>365</v>
       </c>
       <c r="CH14" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="CI14" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="CJ14" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="CK14" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="CL14" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="CI14" s="29" t="s">
+      <c r="CM14" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="CJ14" s="29" t="s">
+      <c r="CN14" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="CK14" s="29" t="s">
+      <c r="CO14" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="CL14" s="57" t="s">
+      <c r="CP14" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="CQ14" s="12" t="s">
         <v>489</v>
-      </c>
-      <c r="CM14" s="57" t="s">
-        <v>489</v>
-      </c>
-      <c r="CN14" s="57" t="s">
-        <v>489</v>
-      </c>
-      <c r="CO14" s="57" t="s">
-        <v>489</v>
-      </c>
-      <c r="CP14" s="57" t="s">
-        <v>487</v>
-      </c>
-      <c r="CQ14" s="12" t="s">
-        <v>490</v>
       </c>
       <c r="CR14" s="62">
         <v>44227.0</v>
@@ -11973,7 +11970,7 @@
         <v>389</v>
       </c>
       <c r="CV14" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="CW14" s="12" t="s">
         <v>365</v>
@@ -12011,15 +12008,15 @@
       <c r="DX14" s="64"/>
       <c r="DY14" s="64"/>
       <c r="DZ14" s="66" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" ht="16.5" customHeight="1">
       <c r="A15" s="56" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>365</v>
@@ -12028,7 +12025,7 @@
         <v>363</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>365</v>
@@ -12049,16 +12046,16 @@
         <v>1002.0</v>
       </c>
       <c r="L15" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N15" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="M15" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N15" s="12" t="s">
+      <c r="O15" s="12" t="s">
         <v>496</v>
-      </c>
-      <c r="O15" s="12" t="s">
-        <v>497</v>
       </c>
       <c r="P15" s="60" t="s">
         <v>371</v>
@@ -12124,7 +12121,7 @@
         <v>365</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AL15" s="12">
         <v>8000.0</v>
@@ -12139,7 +12136,7 @@
         <v>80000.0</v>
       </c>
       <c r="AP15" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AQ15" s="12" t="s">
         <v>377</v>
@@ -12166,13 +12163,13 @@
         <v>377</v>
       </c>
       <c r="AY15" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AZ15" s="60" t="s">
         <v>378</v>
       </c>
       <c r="BA15" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="BB15" s="68">
         <v>44197.0</v>
@@ -12202,13 +12199,13 @@
         <v>365</v>
       </c>
       <c r="BK15" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="BL15" s="12">
         <v>1.0</v>
       </c>
       <c r="BM15" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="BN15" s="12" t="s">
         <v>382</v>
@@ -12229,10 +12226,10 @@
         <v>365</v>
       </c>
       <c r="BT15" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="BU15" s="34" t="s">
         <v>504</v>
-      </c>
-      <c r="BU15" s="34" t="s">
-        <v>505</v>
       </c>
       <c r="BV15" s="61" t="s">
         <v>373</v>
@@ -12271,34 +12268,34 @@
         <v>365</v>
       </c>
       <c r="CH15" s="69" t="s">
+        <v>505</v>
+      </c>
+      <c r="CI15" s="69" t="s">
+        <v>505</v>
+      </c>
+      <c r="CJ15" s="69" t="s">
+        <v>505</v>
+      </c>
+      <c r="CK15" s="69" t="s">
+        <v>505</v>
+      </c>
+      <c r="CL15" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="CI15" s="69" t="s">
+      <c r="CM15" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="CJ15" s="69" t="s">
+      <c r="CN15" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="CK15" s="69" t="s">
+      <c r="CO15" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="CL15" s="57" t="s">
+      <c r="CP15" s="57" t="s">
+        <v>504</v>
+      </c>
+      <c r="CQ15" s="12" t="s">
         <v>507</v>
-      </c>
-      <c r="CM15" s="57" t="s">
-        <v>507</v>
-      </c>
-      <c r="CN15" s="57" t="s">
-        <v>507</v>
-      </c>
-      <c r="CO15" s="57" t="s">
-        <v>507</v>
-      </c>
-      <c r="CP15" s="57" t="s">
-        <v>505</v>
-      </c>
-      <c r="CQ15" s="12" t="s">
-        <v>508</v>
       </c>
       <c r="CR15" s="62">
         <v>43861.0</v>
@@ -12325,26 +12322,26 @@
         <v>365</v>
       </c>
       <c r="CZ15" s="40" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="DA15" s="64"/>
       <c r="DB15" s="40" t="s">
+        <v>509</v>
+      </c>
+      <c r="DC15" s="40" t="s">
         <v>510</v>
       </c>
-      <c r="DC15" s="40" t="s">
+      <c r="DD15" s="40" t="s">
         <v>511</v>
-      </c>
-      <c r="DD15" s="40" t="s">
-        <v>512</v>
       </c>
       <c r="DE15" s="40" t="s">
         <v>378</v>
       </c>
       <c r="DF15" s="40" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="DG15" s="40" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="DH15" s="40" t="s">
         <v>389</v>
@@ -12353,19 +12350,19 @@
         <v>382</v>
       </c>
       <c r="DJ15" s="40" t="s">
+        <v>513</v>
+      </c>
+      <c r="DK15" s="40" t="s">
+        <v>513</v>
+      </c>
+      <c r="DL15" s="40" t="s">
+        <v>513</v>
+      </c>
+      <c r="DM15" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="DN15" s="40" t="s">
         <v>514</v>
-      </c>
-      <c r="DK15" s="40" t="s">
-        <v>514</v>
-      </c>
-      <c r="DL15" s="40" t="s">
-        <v>514</v>
-      </c>
-      <c r="DM15" s="12" t="s">
-        <v>514</v>
-      </c>
-      <c r="DN15" s="40" t="s">
-        <v>515</v>
       </c>
       <c r="DO15" s="64"/>
       <c r="DP15" s="40" t="s">
@@ -12373,7 +12370,7 @@
       </c>
       <c r="DQ15" s="64"/>
       <c r="DR15" s="40" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="DS15" s="64"/>
       <c r="DT15" s="64"/>
@@ -12386,10 +12383,10 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="56" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>365</v>
@@ -12398,7 +12395,7 @@
         <v>363</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>365</v>
@@ -12419,16 +12416,16 @@
         <v>1003.0</v>
       </c>
       <c r="L16" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N16" s="12" t="s">
         <v>518</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N16" s="12" t="s">
+      <c r="O16" s="57" t="s">
         <v>519</v>
-      </c>
-      <c r="O16" s="57" t="s">
-        <v>520</v>
       </c>
       <c r="P16" s="60" t="s">
         <v>371</v>
@@ -12494,7 +12491,7 @@
         <v>365</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AL16" s="12">
         <v>8999.0</v>
@@ -12509,7 +12506,7 @@
         <v>90000.0</v>
       </c>
       <c r="AP16" s="12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AQ16" s="12" t="s">
         <v>374</v>
@@ -12536,13 +12533,13 @@
         <v>374</v>
       </c>
       <c r="AY16" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="AZ16" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="BA16" s="12" t="s">
         <v>522</v>
-      </c>
-      <c r="AZ16" s="60" t="s">
-        <v>421</v>
-      </c>
-      <c r="BA16" s="12" t="s">
-        <v>523</v>
       </c>
       <c r="BB16" s="62">
         <v>44562.0</v>
@@ -12572,16 +12569,16 @@
         <v>365</v>
       </c>
       <c r="BK16" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="BL16" s="12">
         <v>3.0</v>
       </c>
       <c r="BM16" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="BN16" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BO16" s="12" t="s">
         <v>365</v>
@@ -12599,10 +12596,10 @@
         <v>365</v>
       </c>
       <c r="BT16" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="BU16" s="34" t="s">
         <v>526</v>
-      </c>
-      <c r="BU16" s="34" t="s">
-        <v>527</v>
       </c>
       <c r="BV16" s="61" t="s">
         <v>373</v>
@@ -12641,34 +12638,34 @@
         <v>365</v>
       </c>
       <c r="CH16" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="CI16" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="CJ16" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="CK16" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="CL16" s="57" t="s">
         <v>528</v>
       </c>
-      <c r="CI16" s="69" t="s">
+      <c r="CM16" s="57" t="s">
         <v>528</v>
       </c>
-      <c r="CJ16" s="69" t="s">
+      <c r="CN16" s="57" t="s">
         <v>528</v>
       </c>
-      <c r="CK16" s="69" t="s">
+      <c r="CO16" s="57" t="s">
         <v>528</v>
       </c>
-      <c r="CL16" s="57" t="s">
+      <c r="CP16" s="57" t="s">
+        <v>526</v>
+      </c>
+      <c r="CQ16" s="12" t="s">
         <v>529</v>
-      </c>
-      <c r="CM16" s="57" t="s">
-        <v>529</v>
-      </c>
-      <c r="CN16" s="57" t="s">
-        <v>529</v>
-      </c>
-      <c r="CO16" s="57" t="s">
-        <v>529</v>
-      </c>
-      <c r="CP16" s="57" t="s">
-        <v>527</v>
-      </c>
-      <c r="CQ16" s="12" t="s">
-        <v>530</v>
       </c>
       <c r="CR16" s="62">
         <v>44227.0</v>
@@ -12680,7 +12677,7 @@
         <v>366</v>
       </c>
       <c r="CU16" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="CV16" s="12" t="s">
         <v>365</v>
@@ -12724,10 +12721,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="56" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C17" s="70"/>
       <c r="D17" s="70"/>
@@ -12860,10 +12857,10 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="56" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C18" s="70"/>
       <c r="D18" s="70"/>
@@ -41265,7 +41262,7 @@
       <c r="B5" s="75"/>
       <c r="C5" s="76"/>
       <c r="D5" s="50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E5" s="76"/>
     </row>
@@ -42923,7 +42920,7 @@
         <v>345</v>
       </c>
       <c r="AE3" s="51" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4">
@@ -42931,7 +42928,7 @@
         <v>350</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>
@@ -43066,16 +43063,16 @@
         <v>373</v>
       </c>
       <c r="J7" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>537</v>
-      </c>
       <c r="M7" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>365</v>
@@ -43105,10 +43102,10 @@
         <v>381</v>
       </c>
       <c r="W7" s="60" t="s">
+        <v>537</v>
+      </c>
+      <c r="X7" s="12" t="s">
         <v>538</v>
-      </c>
-      <c r="X7" s="12" t="s">
-        <v>539</v>
       </c>
       <c r="Y7" s="12" t="s">
         <v>365</v>
@@ -43126,10 +43123,10 @@
         <v>375</v>
       </c>
       <c r="AD7" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE7" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -43167,10 +43164,10 @@
         <v>365</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>365</v>
@@ -43200,10 +43197,10 @@
         <v>381</v>
       </c>
       <c r="W8" s="60" t="s">
+        <v>537</v>
+      </c>
+      <c r="X8" s="12" t="s">
         <v>538</v>
-      </c>
-      <c r="X8" s="12" t="s">
-        <v>539</v>
       </c>
       <c r="Y8" s="12" t="s">
         <v>365</v>
@@ -43221,10 +43218,10 @@
         <v>375</v>
       </c>
       <c r="AD8" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE8" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -43256,16 +43253,16 @@
         <v>373</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="N9" s="12" t="s">
         <v>365</v>
@@ -43283,7 +43280,7 @@
         <v>365</v>
       </c>
       <c r="S9" s="57" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="T9" s="12" t="s">
         <v>365</v>
@@ -43292,13 +43289,13 @@
         <v>395</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W9" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="X9" s="12" t="s">
         <v>542</v>
-      </c>
-      <c r="X9" s="12" t="s">
-        <v>543</v>
       </c>
       <c r="Y9" s="12" t="s">
         <v>365</v>
@@ -43316,10 +43313,10 @@
         <v>375</v>
       </c>
       <c r="AD9" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AE9" s="60" t="s">
         <v>544</v>
-      </c>
-      <c r="AE9" s="60" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -43345,22 +43342,22 @@
         <v>375</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I10" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>365</v>
@@ -43378,7 +43375,7 @@
         <v>365</v>
       </c>
       <c r="S10" s="57" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="T10" s="12" t="s">
         <v>365</v>
@@ -43387,13 +43384,13 @@
         <v>395</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W10" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="X10" s="12" t="s">
         <v>542</v>
-      </c>
-      <c r="X10" s="12" t="s">
-        <v>543</v>
       </c>
       <c r="Y10" s="12" t="s">
         <v>365</v>
@@ -43411,21 +43408,21 @@
         <v>375</v>
       </c>
       <c r="AD10" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AE10" s="60" t="s">
         <v>544</v>
-      </c>
-      <c r="AE10" s="60" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B11" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>365</v>
@@ -43446,49 +43443,49 @@
         <v>373</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L11" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="R11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="S11" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="U11" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="W11" s="60" t="s">
         <v>548</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="R11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="S11" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="U11" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="V11" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="W11" s="60" t="s">
+      <c r="X11" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X11" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y11" s="12" t="s">
         <v>365</v>
@@ -43506,21 +43503,21 @@
         <v>375</v>
       </c>
       <c r="AD11" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="AE11" s="60" t="s">
         <v>551</v>
-      </c>
-      <c r="AE11" s="60" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B12" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>365</v>
@@ -43535,55 +43532,55 @@
         <v>365</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I12" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J12" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="L12" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="S12" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="W12" s="60" t="s">
         <v>548</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="S12" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="V12" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="W12" s="60" t="s">
+      <c r="X12" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X12" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y12" s="12" t="s">
         <v>365</v>
@@ -43601,21 +43598,21 @@
         <v>375</v>
       </c>
       <c r="AD12" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="AE12" s="60" t="s">
         <v>551</v>
-      </c>
-      <c r="AE12" s="60" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="56" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B13" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>365</v>
@@ -43636,16 +43633,16 @@
         <v>373</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>365</v>
@@ -43663,22 +43660,22 @@
         <v>365</v>
       </c>
       <c r="S13" s="57" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T13" s="12" t="s">
         <v>365</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="W13" s="60" t="s">
+        <v>537</v>
+      </c>
+      <c r="X13" s="12" t="s">
         <v>538</v>
-      </c>
-      <c r="X13" s="12" t="s">
-        <v>539</v>
       </c>
       <c r="Y13" s="12" t="s">
         <v>365</v>
@@ -43696,21 +43693,21 @@
         <v>375</v>
       </c>
       <c r="AD13" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE13" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="56" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B14" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>365</v>
@@ -43725,22 +43722,22 @@
         <v>365</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I14" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>365</v>
@@ -43758,22 +43755,22 @@
         <v>365</v>
       </c>
       <c r="S14" s="57" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V14" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="W14" s="60" t="s">
+        <v>537</v>
+      </c>
+      <c r="X14" s="12" t="s">
         <v>538</v>
-      </c>
-      <c r="X14" s="12" t="s">
-        <v>539</v>
       </c>
       <c r="Y14" s="12" t="s">
         <v>365</v>
@@ -43791,21 +43788,21 @@
         <v>375</v>
       </c>
       <c r="AD14" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE14" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="56" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B15" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>365</v>
@@ -43826,16 +43823,16 @@
         <v>373</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>365</v>
@@ -43853,22 +43850,22 @@
         <v>365</v>
       </c>
       <c r="S15" s="57" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T15" s="12" t="s">
         <v>365</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="V15" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="W15" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="X15" s="12" t="s">
         <v>542</v>
-      </c>
-      <c r="X15" s="12" t="s">
-        <v>543</v>
       </c>
       <c r="Y15" s="12" t="s">
         <v>365</v>
@@ -43886,21 +43883,21 @@
         <v>375</v>
       </c>
       <c r="AD15" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="AE15" s="60" t="s">
         <v>551</v>
-      </c>
-      <c r="AE15" s="60" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="56" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B16" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>365</v>
@@ -43915,22 +43912,22 @@
         <v>365</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I16" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>365</v>
@@ -43948,22 +43945,22 @@
         <v>365</v>
       </c>
       <c r="S16" s="57" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="V16" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="W16" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="X16" s="12" t="s">
         <v>542</v>
-      </c>
-      <c r="X16" s="12" t="s">
-        <v>543</v>
       </c>
       <c r="Y16" s="12" t="s">
         <v>365</v>
@@ -43981,21 +43978,21 @@
         <v>375</v>
       </c>
       <c r="AD16" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="AE16" s="60" t="s">
         <v>551</v>
-      </c>
-      <c r="AE16" s="60" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B17" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>365</v>
@@ -44016,16 +44013,16 @@
         <v>373</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>365</v>
@@ -44043,22 +44040,22 @@
         <v>365</v>
       </c>
       <c r="S17" s="57" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="T17" s="12" t="s">
         <v>365</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="V17" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W17" s="60" t="s">
+        <v>548</v>
+      </c>
+      <c r="X17" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X17" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y17" s="12" t="s">
         <v>365</v>
@@ -44076,21 +44073,21 @@
         <v>375</v>
       </c>
       <c r="AD17" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AE17" s="60" t="s">
         <v>544</v>
-      </c>
-      <c r="AE17" s="60" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B18" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>365</v>
@@ -44105,22 +44102,22 @@
         <v>375</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I18" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>365</v>
@@ -44138,22 +44135,22 @@
         <v>365</v>
       </c>
       <c r="S18" s="57" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="T18" s="12" t="s">
         <v>365</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="V18" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W18" s="60" t="s">
+        <v>548</v>
+      </c>
+      <c r="X18" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X18" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y18" s="12" t="s">
         <v>365</v>
@@ -44171,21 +44168,21 @@
         <v>375</v>
       </c>
       <c r="AD18" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AE18" s="60" t="s">
         <v>544</v>
-      </c>
-      <c r="AE18" s="60" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="56" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B19" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>365</v>
@@ -44206,16 +44203,16 @@
         <v>373</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>365</v>
@@ -44233,22 +44230,22 @@
         <v>365</v>
       </c>
       <c r="S19" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="T19" s="12" t="s">
         <v>365</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V19" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="W19" s="60" t="s">
+        <v>548</v>
+      </c>
+      <c r="X19" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X19" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y19" s="12" t="s">
         <v>365</v>
@@ -44266,21 +44263,21 @@
         <v>375</v>
       </c>
       <c r="AD19" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE19" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="56" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B20" s="80" t="s">
         <v>367</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>365</v>
@@ -44295,22 +44292,22 @@
         <v>365</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I20" s="81" t="s">
         <v>373</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>365</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>365</v>
@@ -44328,22 +44325,22 @@
         <v>365</v>
       </c>
       <c r="S20" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V20" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="W20" s="60" t="s">
+        <v>548</v>
+      </c>
+      <c r="X20" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="X20" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="Y20" s="12" t="s">
         <v>365</v>
@@ -44361,10 +44358,10 @@
         <v>375</v>
       </c>
       <c r="AD20" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AE20" s="60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -45828,7 +45825,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C2" s="76"/>
     </row>
@@ -45854,7 +45851,7 @@
       </c>
       <c r="B5" s="75"/>
       <c r="C5" s="82" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -45866,24 +45863,24 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="56" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B7" s="83">
         <v>1002.0</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="56" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B8" s="83">
         <v>1003.0</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -45894,7 +45891,7 @@
         <v>367</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -45905,62 +45902,62 @@
         <v>367</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>367</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="56" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>367</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="56" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>367</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>367</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="56" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>367</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -47387,123 +47384,123 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="84" t="s">
+        <v>569</v>
+      </c>
+      <c r="B1" s="85" t="s">
         <v>570</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="C1" s="85" t="s">
         <v>571</v>
-      </c>
-      <c r="C1" s="85" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="27" t="s">
+        <v>572</v>
+      </c>
+      <c r="B2" s="86" t="s">
         <v>573</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="C2" s="86" t="s">
         <v>574</v>
-      </c>
-      <c r="C2" s="86" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B3" s="86" t="s">
+        <v>575</v>
+      </c>
+      <c r="C3" s="86" t="s">
         <v>576</v>
-      </c>
-      <c r="C3" s="86" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B4" s="86" t="s">
+        <v>577</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>578</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B5" s="86" t="s">
+        <v>579</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>580</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B6" s="86" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="86" t="s">
         <v>582</v>
-      </c>
-      <c r="C6" s="86" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B7" s="86" t="s">
+        <v>583</v>
+      </c>
+      <c r="C7" s="86" t="s">
         <v>584</v>
-      </c>
-      <c r="C7" s="86" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B8" s="86" t="s">
+        <v>585</v>
+      </c>
+      <c r="C8" s="86" t="s">
         <v>586</v>
-      </c>
-      <c r="C8" s="86" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B9" s="86" t="s">
+        <v>587</v>
+      </c>
+      <c r="C9" s="86" t="s">
         <v>588</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B10" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="C10" s="69" t="s">
         <v>590</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>591</v>
+      </c>
+      <c r="C11" s="69" t="s">
         <v>592</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
@@ -47511,54 +47508,54 @@
         <v>28</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>594</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B13" s="40" t="s">
+        <v>595</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>596</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B14" s="40" t="s">
+        <v>597</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>598</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B15" s="40" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" s="40" t="s">
         <v>600</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B16" s="40" t="s">
+        <v>601</v>
+      </c>
+      <c r="C16" s="40" t="s">
         <v>602</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
@@ -48558,13 +48555,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="88" t="s">
+        <v>603</v>
+      </c>
+      <c r="B1" s="89" t="s">
         <v>604</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>605</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="2">
@@ -48575,7 +48572,7 @@
         <v>0.0</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3">
@@ -48586,7 +48583,7 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4">
@@ -48597,7 +48594,7 @@
         <v>2.0</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5">
@@ -48608,7 +48605,7 @@
         <v>0.0</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="6">
@@ -48619,40 +48616,40 @@
         <v>1.0</v>
       </c>
       <c r="C6" s="93" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="91" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B7" s="92">
         <v>0.0</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="91" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B8" s="92">
         <v>1.0</v>
       </c>
       <c r="C8" s="91" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="91" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B9" s="92">
         <v>2.0</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10">
@@ -48663,7 +48660,7 @@
         <v>371</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -48695,7 +48692,7 @@
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="44"/>
       <c r="B1" s="45" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>

</xml_diff>